<commit_message>
T11 done for now
</commit_message>
<xml_diff>
--- a/Custom/Custom Items/overview.xlsx
+++ b/Custom/Custom Items/overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Desktop\WoW Server\Azeroth Fork\Custom\Custom Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250A5B6B-F696-4383-A3D2-18F69F1E6328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63818219-84C5-4250-8C55-837C6EE79E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="122">
   <si>
     <t>ID</t>
   </si>
@@ -112,6 +112,288 @@
   </si>
   <si>
     <t>Set ID</t>
+  </si>
+  <si>
+    <t>Sanctified Lasherweave Robes</t>
+  </si>
+  <si>
+    <t>Sanctified Lasherweave Gauntlets</t>
+  </si>
+  <si>
+    <t>Sanctified Lasherweave Helmet</t>
+  </si>
+  <si>
+    <t>Sanctified Lasherweave Legplates</t>
+  </si>
+  <si>
+    <t>Sanctified Lasherweave Pauldrons</t>
+  </si>
+  <si>
+    <t>Sanctified Lasherweave Shoulderpads</t>
+  </si>
+  <si>
+    <t>Sanctified Lasherweave Legguards</t>
+  </si>
+  <si>
+    <t>Sanctified Lasherweave Headguard</t>
+  </si>
+  <si>
+    <t>Sanctified Lasherweave Handgrips</t>
+  </si>
+  <si>
+    <t>Sanctified Lasherweave Raiment</t>
+  </si>
+  <si>
+    <t>Sanctified Lasherweave Mantle</t>
+  </si>
+  <si>
+    <t>Sanctified Lasherweave Trousers</t>
+  </si>
+  <si>
+    <t>Sanctified Lasherweave Cover</t>
+  </si>
+  <si>
+    <t>Sanctified Lasherweave Gloves</t>
+  </si>
+  <si>
+    <t>Sanctified Lasherweave Vestment</t>
+  </si>
+  <si>
+    <t>Sanctified Ahn'Kahar Blood Hunter's Handguards</t>
+  </si>
+  <si>
+    <t>Sanctified Ahn'Kahar Blood Hunter's Headpiece</t>
+  </si>
+  <si>
+    <t>Sanctified Ahn'Kahar Blood Hunter's Legguards</t>
+  </si>
+  <si>
+    <t>Sanctified Ahn'Kahar Blood Hunter's Spaulders</t>
+  </si>
+  <si>
+    <t>Sanctified Ahn'Kahar Blood Hunter's Tunic</t>
+  </si>
+  <si>
+    <t>Sanctified Bloodmage Gloves</t>
+  </si>
+  <si>
+    <t>Sanctified Bloodmage Hood</t>
+  </si>
+  <si>
+    <t>Sanctified Bloodmage Leggings</t>
+  </si>
+  <si>
+    <t>Sanctified Bloodmage Robe</t>
+  </si>
+  <si>
+    <t>Sanctified Bloodmage Shoulderpads</t>
+  </si>
+  <si>
+    <t>Sanctified Lightsworn Shoulderplates</t>
+  </si>
+  <si>
+    <t>Sanctified Lightsworn Legplates</t>
+  </si>
+  <si>
+    <t>Sanctified Lightsworn Helmet</t>
+  </si>
+  <si>
+    <t>Sanctified Lightsworn Gauntlets</t>
+  </si>
+  <si>
+    <t>Sanctified Lightsworn Battleplate</t>
+  </si>
+  <si>
+    <t>Sanctified Lightsworn Shoulderguards</t>
+  </si>
+  <si>
+    <t>Sanctified Lightsworn Legguards</t>
+  </si>
+  <si>
+    <t>Sanctified Lightsworn Handguards</t>
+  </si>
+  <si>
+    <t>Sanctified Lightsworn Faceguard</t>
+  </si>
+  <si>
+    <t>Sanctified Lightsworn Chestguard</t>
+  </si>
+  <si>
+    <t>Sanctified Lightsworn Spaulders</t>
+  </si>
+  <si>
+    <t>Sanctified Lightsworn Tunic</t>
+  </si>
+  <si>
+    <t>Sanctified Lightsworn Headpiece</t>
+  </si>
+  <si>
+    <t>Sanctified Lightsworn Greaves</t>
+  </si>
+  <si>
+    <t>Sanctified Lightsworn Gloves</t>
+  </si>
+  <si>
+    <t>Sanctified Crimson Acolyte Pants</t>
+  </si>
+  <si>
+    <t>Sanctified Crimson Acolyte Raiments</t>
+  </si>
+  <si>
+    <t>Sanctified Crimson Acolyte Mantle</t>
+  </si>
+  <si>
+    <t>Sanctified Crimson Acolyte Handwraps</t>
+  </si>
+  <si>
+    <t>Sanctified Crimson Acolyte Cowl</t>
+  </si>
+  <si>
+    <t>Sanctified Crimson Acolyte Gloves</t>
+  </si>
+  <si>
+    <t>Sanctified Crimson Acolyte Hood</t>
+  </si>
+  <si>
+    <t>Sanctified Crimson Acolyte Leggings</t>
+  </si>
+  <si>
+    <t>Sanctified Crimson Acolyte Robe</t>
+  </si>
+  <si>
+    <t>Sanctified Crimson Acolyte Shoulderpads</t>
+  </si>
+  <si>
+    <t>Sanctified Shadowblade Breastplate</t>
+  </si>
+  <si>
+    <t>Sanctified Shadowblade Gauntlets</t>
+  </si>
+  <si>
+    <t>Sanctified Shadowblade Helmet</t>
+  </si>
+  <si>
+    <t>Sanctified Shadowblade Legplates</t>
+  </si>
+  <si>
+    <t>Sanctified Shadowblade Pauldrons</t>
+  </si>
+  <si>
+    <t>Sanctified Frost Witch's Shoulderguards</t>
+  </si>
+  <si>
+    <t>Sanctified Frost Witch's War-Kilt</t>
+  </si>
+  <si>
+    <t>Sanctified Frost Witch's Faceguard</t>
+  </si>
+  <si>
+    <t>Sanctified Frost Witch's Chestguard</t>
+  </si>
+  <si>
+    <t>Sanctified Frost Witch's Spaulders</t>
+  </si>
+  <si>
+    <t>Sanctified Frost Witch's Legguards</t>
+  </si>
+  <si>
+    <t>Sanctified Frost Witch's Headpiece</t>
+  </si>
+  <si>
+    <t>Sanctified Frost Witch's Handguards</t>
+  </si>
+  <si>
+    <t>Sanctified Frost Witch's Tunic</t>
+  </si>
+  <si>
+    <t>Sanctified Frost Witch's Shoulderpads</t>
+  </si>
+  <si>
+    <t>Sanctified Frost Witch's Kilt</t>
+  </si>
+  <si>
+    <t>Sanctified Frost Witch's Helm</t>
+  </si>
+  <si>
+    <t>Sanctified Frost Witch's Gloves</t>
+  </si>
+  <si>
+    <t>Sanctified Frost Witch's Hauberk</t>
+  </si>
+  <si>
+    <t>Sanctified Dark Coven Gloves</t>
+  </si>
+  <si>
+    <t>Sanctified Dark Coven Hood</t>
+  </si>
+  <si>
+    <t>Sanctified Dark Coven Leggings</t>
+  </si>
+  <si>
+    <t>Sanctified Dark Coven Robe</t>
+  </si>
+  <si>
+    <t>Sanctified Dark Coven Shoulderpads</t>
+  </si>
+  <si>
+    <t>Sanctified Ymirjar Lord's Battleplate</t>
+  </si>
+  <si>
+    <t>Sanctified Ymirjar Lord's Gauntlets</t>
+  </si>
+  <si>
+    <t>Sanctified Ymirjar Lord's Helmet</t>
+  </si>
+  <si>
+    <t>Sanctified Ymirjar Lord's Legplates</t>
+  </si>
+  <si>
+    <t>Sanctified Ymirjar Lord's Shoulderplates</t>
+  </si>
+  <si>
+    <t>Sanctified Ymirjar Lord's Breastplate</t>
+  </si>
+  <si>
+    <t>Sanctified Ymirjar Lord's Greathelm</t>
+  </si>
+  <si>
+    <t>Sanctified Ymirjar Lord's Handguards</t>
+  </si>
+  <si>
+    <t>Sanctified Ymirjar Lord's Legguards</t>
+  </si>
+  <si>
+    <t>Sanctified Ymirjar Lord's Pauldrons</t>
+  </si>
+  <si>
+    <t>Sanctified Frost Witch's Grips</t>
+  </si>
+  <si>
+    <t>Druid</t>
+  </si>
+  <si>
+    <t>Hunter</t>
+  </si>
+  <si>
+    <t>Mage</t>
+  </si>
+  <si>
+    <t>Paladin</t>
+  </si>
+  <si>
+    <t>Priest</t>
+  </si>
+  <si>
+    <t>Rogue</t>
+  </si>
+  <si>
+    <t>Shaman</t>
+  </si>
+  <si>
+    <t>Warlock</t>
+  </si>
+  <si>
+    <t>Warrior</t>
   </si>
 </sst>
 </file>
@@ -460,16 +742,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="H99" sqref="H99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.90625" customWidth="1"/>
-    <col min="2" max="2" width="37.36328125" customWidth="1"/>
+    <col min="2" max="2" width="41.90625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="47.90625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -784,174 +1066,2044 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="1">
+        <v>81010</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1002</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="A15" s="1">
+        <v>81011</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1002</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="A16" s="1">
+        <v>81012</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1002</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="A17" s="1">
+        <v>81013</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1002</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="A18" s="1">
+        <v>81014</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1002</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="A19" s="1">
+        <v>81015</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1003</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="A20" s="1">
+        <v>81016</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1003</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="A21" s="1">
+        <v>81017</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1003</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="A22" s="1">
+        <v>81018</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1003</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="A23" s="1">
+        <v>81019</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1003</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="A24" s="1">
+        <v>81020</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1004</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="A25" s="1">
+        <v>81021</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1004</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="A26" s="1">
+        <v>81022</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1004</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="A27" s="1">
+        <v>81023</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1004</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="A28" s="1">
+        <v>81024</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1004</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="A29" s="1">
+        <v>81025</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1005</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="A30" s="1">
+        <v>81026</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
+      <c r="E30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1005</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>81027</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1005</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>81028</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1005</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>81029</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1005</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>81030</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1006</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>81031</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1006</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <v>81032</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1006</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>81033</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1006</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>81034</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1006</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" s="1">
+        <v>81035</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1007</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" s="1">
+        <v>81036</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1007</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" s="1">
+        <v>81037</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" s="1">
+        <v>1007</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" s="1">
+        <v>81038</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1007</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" s="1">
+        <v>81039</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F43" s="1">
+        <v>1007</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" s="1">
+        <v>81040</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1008</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" s="1">
+        <v>81041</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F45" s="1">
+        <v>1008</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" s="1">
+        <v>81042</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F46" s="1">
+        <v>1008</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" s="1">
+        <v>81043</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F47" s="1">
+        <v>1008</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" s="1">
+        <v>81044</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" s="1">
+        <v>1008</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" s="1">
+        <v>81045</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F49" s="1">
+        <v>1009</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" s="1">
+        <v>81046</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50" s="1">
+        <v>1009</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" s="1">
+        <v>81047</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" s="1">
+        <v>1009</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" s="1">
+        <v>81048</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F52" s="1">
+        <v>1009</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" s="1">
+        <v>81049</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F53" s="1">
+        <v>1009</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" s="1">
+        <v>81050</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F54" s="1">
+        <v>1010</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55" s="1">
+        <v>81051</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F55" s="1">
+        <v>1010</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" s="1">
+        <v>81052</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F56" s="1">
+        <v>1010</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57" s="1">
+        <v>81053</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F57" s="1">
+        <v>1010</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58" s="1">
+        <v>81054</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F58" s="1">
+        <v>1010</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A59" s="1">
+        <v>81055</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F59" s="1">
+        <v>1011</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A60" s="1">
+        <v>81056</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F60" s="1">
+        <v>1011</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A61" s="1">
+        <v>81057</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1011</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A62" s="1">
+        <v>81058</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F62" s="1">
+        <v>1011</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63" s="1">
+        <v>81059</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F63" s="1">
+        <v>1011</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A64" s="1">
+        <v>81060</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F64" s="1">
+        <v>1012</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A65" s="1">
+        <v>81061</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F65" s="1">
+        <v>1012</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66" s="1">
+        <v>81062</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F66" s="1">
+        <v>1012</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A67" s="1">
+        <v>81063</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F67" s="1">
+        <v>1012</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A68" s="1">
+        <v>81064</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F68" s="1">
+        <v>1012</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A69" s="1">
+        <v>81065</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F69" s="1">
+        <v>1013</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A70" s="1">
+        <v>81066</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F70" s="1">
+        <v>1013</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A71" s="1">
+        <v>81067</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F71" s="1">
+        <v>1013</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A72" s="1">
+        <v>81068</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F72" s="1">
+        <v>1013</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A73" s="1">
+        <v>81069</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F73" s="1">
+        <v>1013</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A74" s="1">
+        <v>81070</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F74" s="1">
+        <v>1014</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A75" s="1">
+        <v>81071</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F75" s="1">
+        <v>1014</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A76" s="1">
+        <v>81072</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F76" s="1">
+        <v>1014</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A77" s="1">
+        <v>81073</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F77" s="1">
+        <v>1014</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A78" s="1">
+        <v>81074</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F78" s="1">
+        <v>1014</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A79" s="1">
+        <v>81075</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F79" s="1">
+        <v>1015</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A80" s="1">
+        <v>81076</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F80" s="1">
+        <v>1015</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A81" s="1">
+        <v>81077</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F81" s="1">
+        <v>1015</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A82" s="1">
+        <v>81078</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F82" s="1">
+        <v>1015</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A83" s="1">
+        <v>81079</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F83" s="1">
+        <v>1015</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A84" s="1">
+        <v>81080</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F84" s="1">
+        <v>1016</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A85" s="1">
+        <v>81081</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F85" s="1">
+        <v>1016</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A86" s="1">
+        <v>81082</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F86" s="1">
+        <v>1016</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A87" s="1">
+        <v>81083</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F87" s="1">
+        <v>1016</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A88" s="1">
+        <v>81084</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F88" s="1">
+        <v>1016</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A89" s="1">
+        <v>81085</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F89" s="1">
+        <v>1017</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A90" s="1">
+        <v>81086</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F90" s="1">
+        <v>1017</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A91" s="1">
+        <v>81087</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F91" s="1">
+        <v>1017</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A92" s="1">
+        <v>81088</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F92" s="1">
+        <v>1017</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A93" s="1">
+        <v>81089</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F93" s="1">
+        <v>1017</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A94" s="1">
+        <v>81090</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F94" s="1">
+        <v>1018</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A95" s="1">
+        <v>81091</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F95" s="1">
+        <v>1018</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A96" s="1">
+        <v>81092</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F96" s="1">
+        <v>1018</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A97" s="1">
+        <v>81093</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F97" s="1">
+        <v>1018</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A98" s="1">
+        <v>81094</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F98" s="1">
+        <v>1018</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>